<commit_message>
Enabled macro to do paste as values only
</commit_message>
<xml_diff>
--- a/sequencing_metadata.xlsx
+++ b/sequencing_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vincent.tu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://phila-my.sharepoint.com/personal/vincent_tu_phila_gov/Documents/git/MetadataSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE80E38-DB7E-4676-88FD-2CA4AAD9682A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{8BE80E38-DB7E-4676-88FD-2CA4AAD9682A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C4552E-B0D2-45F7-A788-93425F2C110A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1458,7 +1458,70 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7DA5BBF6-035D-F947-8AEE-5FE695C8F9E9}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{35A482AB-CB53-3941-A9D9-CA0EA079F9B7}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1865,7 +1928,7 @@
   <dimension ref="A1:AE962"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
@@ -1956,6 +2019,7 @@
       <c r="AA1" s="13"/>
     </row>
     <row r="2" spans="1:31" s="27" customFormat="1">
+      <c r="A2" s="45"/>
       <c r="B2" s="44" t="s">
         <v>63</v>
       </c>
@@ -1995,6 +2059,7 @@
       <c r="AA2" s="31"/>
     </row>
     <row r="3" spans="1:31" s="28" customFormat="1">
+      <c r="A3" s="45"/>
       <c r="B3" s="44" t="s">
         <v>67</v>
       </c>
@@ -2034,6 +2099,7 @@
       <c r="AE3" s="29"/>
     </row>
     <row r="4" spans="1:31">
+      <c r="A4" s="45"/>
       <c r="B4" s="44" t="s">
         <v>69</v>
       </c>
@@ -2712,6 +2778,7 @@
       <c r="Z20" s="44"/>
     </row>
     <row r="21" spans="1:26">
+      <c r="A21" s="45"/>
       <c r="B21" s="44" t="s">
         <v>71</v>
       </c>
@@ -2750,6 +2817,7 @@
       <c r="Z21" s="44"/>
     </row>
     <row r="22" spans="1:26">
+      <c r="A22" s="45"/>
       <c r="B22" s="44" t="s">
         <v>72</v>
       </c>
@@ -2788,6 +2856,7 @@
       <c r="Z22" s="44"/>
     </row>
     <row r="23" spans="1:26">
+      <c r="A23" s="45"/>
       <c r="B23" s="44" t="s">
         <v>73</v>
       </c>
@@ -32525,29 +32594,44 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="B2:Z5 A5 A24:Z961 B21:Z23 A6:Z20">
-    <cfRule type="containsBlanks" dxfId="4" priority="40" stopIfTrue="1">
+  <conditionalFormatting sqref="A24:Z961 B21:Z23 A2:Z20">
+    <cfRule type="containsBlanks" dxfId="7" priority="43" stopIfTrue="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I961 M2:M961 O2:O961 Q2:Z961">
-    <cfRule type="expression" dxfId="3" priority="91">
+    <cfRule type="expression" dxfId="6" priority="94">
       <formula>NOT(ISNUMBER(SUMPRODUCT(FIND(MID(I2,ROW(INDIRECT("1:"&amp;LEN(I2))),1),allowedGeneral))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F961">
-    <cfRule type="expression" dxfId="2" priority="44">
+    <cfRule type="expression" dxfId="5" priority="47">
       <formula>NOT(ISNUMBER(MATCH(F2,allowedSampleTypes,0)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A24:A961 A5:A20">
-    <cfRule type="expression" dxfId="1" priority="98">
-      <formula>ISNUMBER(FIND(LEFT(A5,1),"1234567890"))</formula>
+  <conditionalFormatting sqref="A2:A961">
+    <cfRule type="expression" dxfId="4" priority="101">
+      <formula>ISNUMBER(FIND(LEFT(A2,1),"1234567890"))</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="102"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="containsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A21))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="containsBlanks" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>LEN(TRIM(A22))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>LEN(TRIM(A23))=0</formula>
+    </cfRule>
   </conditionalFormatting>
   <dataValidations count="9">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid entry" error="Your entry contains invalid characters. Please see the &quot;AllowedCharacters&quot; worksheet for more info." sqref="Q3:Z1048576 AA962:AB1048576 I2:I961 D2:D961 M2:M961 O2:O961 Q2:Z2" xr:uid="{D9A1C3E9-8F40-0841-ABF6-7B7371CBD0E2}">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid entry" error="Your entry contains invalid characters. Please see the &quot;AllowedCharacters&quot; worksheet for more info." sqref="AA962:AB1048576 I2:I961 D2:D961 M2:M961 O2:O961 Q2:Z1048576" xr:uid="{D9A1C3E9-8F40-0841-ABF6-7B7371CBD0E2}">
       <formula1>ISNUMBER(SUMPRODUCT(FIND(MID(D2,ROW(INDIRECT("1:"&amp;LEN(D2))),1),allowedGeneral)))</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Column Name" error="Your column name contains invalid characters. Please see allowed characters in the &quot;AllowedCharacters&quot; worksheet." sqref="A1:Z1" xr:uid="{7F3449FB-140F-D544-BCBD-0CBAC5E46220}">
@@ -32572,8 +32656,8 @@
     <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid entry" error="The run column can only contain numbers. Please consult the AllowedCharacters sheet for approved digits for this column" sqref="P2:P961" xr:uid="{E800B48F-B7AB-4AC7-8310-E507A6CAA180}">
       <formula1>ISNUMBER(SUMPRODUCT(FIND(MID(P2,ROW(INDIRECT("1:"&amp;LEN(P2))),1),allowedNumbers)))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid entry" error="Your SampleID contains incorrect characters or is a duplicate. Please only use characters in the AllowedCharacters worksheet. Do not begin SampleID's with a number." sqref="A24:A961 A5:A20" xr:uid="{478ADBF3-907B-4B4D-B5F4-25B5529EE546}">
-      <formula1>AND(ISNUMBER(SUMPRODUCT(FIND(MID(A5,ROW(INDIRECT("1:"&amp;LEN(A5))),1),allowedSampleID))),NOT(ISNUMBER(FIND(LEFT(A5,1),"1234567890"))),COUNTIF($A$1:$A$961, A5)&lt;=1)</formula1>
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid entry" error="Your SampleID contains incorrect characters or is a duplicate. Please only use characters in the AllowedCharacters worksheet. Do not begin SampleID's with a number." sqref="A2:A961" xr:uid="{478ADBF3-907B-4B4D-B5F4-25B5529EE546}">
+      <formula1>AND(ISNUMBER(SUMPRODUCT(FIND(MID(A2,ROW(INDIRECT("1:"&amp;LEN(A2))),1),allowedSampleID))),NOT(ISNUMBER(FIND(LEFT(A2,1),"1234567890"))),COUNTIF($A$1:$A$961, A2)&lt;=1)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>